<commit_message>
update quote and backtest pages
</commit_message>
<xml_diff>
--- a/天朗1月.xlsx
+++ b/天朗1月.xlsx
@@ -1429,13 +1429,14 @@
   <sheetPr/>
   <dimension ref="A1:AB91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="21.7884615384615" customWidth="1"/>
+    <col min="3" max="3" width="13.7788461538462" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="34" spans="1:28">

</xml_diff>